<commit_message>
Statistic: Polynomial Regression - Worksheet
</commit_message>
<xml_diff>
--- a/python/trend/61-poly-regs.xlsx
+++ b/python/trend/61-poly-regs.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">T-value and p-value</t>
+    <t xml:space="preserve">t-value and p-value</t>
   </si>
   <si>
     <t xml:space="preserve">t-value</t>
@@ -283,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -331,17 +331,20 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin">
-        <color rgb="FF009688"/>
-      </right>
+      <right/>
       <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF009688"/>
-      </left>
+      <left/>
       <right style="thin">
         <color rgb="FF009688"/>
       </right>
@@ -355,20 +358,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -427,7 +416,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,31 +505,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,15 +545,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,35 +565,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -608,19 +589,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,7 +691,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="coeff_1" displayName="coeff_1" ref="I8:I9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="coeff_1" displayName="coeff_1" ref="J8:J9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -714,7 +699,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="coeff_2" displayName="coeff_2" ref="L7:L9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="coeff_2" displayName="coeff_2" ref="M7:M9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -722,7 +707,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="coeff_3" displayName="coeff_3" ref="O6:O9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="coeff_3" displayName="coeff_3" ref="P6:P9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -730,7 +715,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="x_observed" displayName="x_observed" ref="B41:B53" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="x_observed" displayName="x_observed" ref="B43:B55" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -738,7 +723,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="y1_predicted" displayName="y1_predicted" ref="E41:E53" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="y1_predicted" displayName="y1_predicted" ref="E43:E55" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -746,7 +731,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="y2_predicted" displayName="y2_predicted" ref="F41:F53" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="y2_predicted" displayName="y2_predicted" ref="G43:G55" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -754,7 +739,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="y3_predicted" displayName="y3_predicted" ref="G41:G53" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="y3_predicted" displayName="y3_predicted" ref="H43:H55" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -762,7 +747,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="y_observed" displayName="y_observed" ref="C41:C53" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="y_observed" displayName="y_observed" ref="C43:C55" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>
@@ -881,10 +866,10 @@
     <tabColor rgb="FF90CAF9"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -892,15 +877,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="15.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="15.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="12.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="12.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="2" width="12.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="2" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="2" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="2.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -908,7 +895,7 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -917,1120 +904,1163 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-      <c r="F5" s="5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="5"/>
+      <c r="J5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="0"/>
-      <c r="O6" s="9" t="n">
-        <f aca="false" t="array" ref="O6:P9">TRANSPOSE(LINEST(C41:C53,B41:B53^{1,2,3},1,1))</f>
+      <c r="P6" s="9" t="n">
+        <f aca="false" t="array" ref="P6:Q9">TRANSPOSE(LINEST(y_observed,x_observed^{1,2,3},1,1))</f>
         <v>2</v>
       </c>
-      <c r="P6" s="9" t="n">
+      <c r="Q6" s="9" t="n">
         <v>2.42035633856246E-015</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="0"/>
-      <c r="L7" s="9" t="n">
-        <f aca="false" t="array" ref="L7:M9">TRANSPOSE(LINEST(C41:C53,B41:B53^{1,2},1,1))</f>
+      <c r="M7" s="9" t="n">
+        <f aca="false" t="array" ref="M7:N9">TRANSPOSE(LINEST(y_observed,x_observed^{1,2},1,1))</f>
         <v>39</v>
       </c>
-      <c r="M7" s="9" t="n">
+      <c r="N7" s="9" t="n">
         <v>2.02837021134844</v>
       </c>
-      <c r="O7" s="11" t="n">
+      <c r="P7" s="11" t="n">
         <v>2.99999999999999</v>
       </c>
-      <c r="P7" s="11" t="n">
+      <c r="Q7" s="11" t="n">
         <v>4.42525415656703E-014</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="0"/>
-      <c r="I8" s="13" t="n">
-        <f aca="false" t="array" ref="I8:J9">TRANSPOSE(LINEST(C41:C53,B41:B53,1,1))</f>
+      <c r="J8" s="13" t="n">
+        <f aca="false" t="array" ref="J8:K9">TRANSPOSE(LINEST(y_observed,x_observed,1,1))</f>
         <v>306</v>
       </c>
-      <c r="J8" s="13" t="n">
+      <c r="K8" s="13" t="n">
         <v>39.5239529544156</v>
       </c>
-      <c r="L8" s="11" t="n">
+      <c r="M8" s="11" t="n">
         <v>-162</v>
       </c>
-      <c r="M8" s="11" t="n">
+      <c r="N8" s="11" t="n">
         <v>25.2530054788392</v>
       </c>
-      <c r="O8" s="11" t="n">
+      <c r="P8" s="11" t="n">
         <v>4.00000000000001</v>
       </c>
-      <c r="P8" s="11" t="n">
+      <c r="Q8" s="11" t="n">
         <v>2.22926325219824E-013</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="0"/>
-      <c r="I9" s="15" t="n">
+      <c r="J9" s="15" t="n">
         <v>-721</v>
       </c>
-      <c r="J9" s="15" t="n">
+      <c r="K9" s="15" t="n">
         <v>279.476551533654</v>
       </c>
-      <c r="L9" s="11" t="n">
+      <c r="M9" s="11" t="n">
         <v>137</v>
       </c>
-      <c r="M9" s="11" t="n">
+      <c r="N9" s="11" t="n">
         <v>65.2240096020738</v>
       </c>
-      <c r="O9" s="11" t="n">
+      <c r="P9" s="11" t="n">
         <v>5.00000000000023</v>
       </c>
-      <c r="P9" s="11" t="n">
+      <c r="Q9" s="11" t="n">
         <v>2.96347194327798E-013</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="H10" s="0"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="5" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="5"/>
+      <c r="J11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="M11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="N11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="P11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P11" s="16" t="s">
+      <c r="Q11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="Q11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
-      <c r="J12" s="17"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="18"/>
-      <c r="O12" s="19" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="K12" s="17"/>
+      <c r="N12" s="18"/>
+      <c r="P12" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="18" t="n">
-        <f aca="false">O6/P6</f>
+      <c r="Q12" s="18" t="n">
+        <f aca="false">P6/Q6</f>
         <v>826324606891509</v>
       </c>
-      <c r="Q12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
-      <c r="J13" s="17"/>
-      <c r="L13" s="20" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="K13" s="17"/>
+      <c r="M13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="18" t="n">
-        <f aca="false">L7/M7</f>
+      <c r="N13" s="18" t="n">
+        <f aca="false">M7/N7</f>
         <v>19.2272592950738</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="P13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P13" s="18" t="n">
-        <f aca="false">O7/P7</f>
+      <c r="Q13" s="18" t="n">
+        <f aca="false">P7/Q7</f>
         <v>67792716392300.8</v>
       </c>
-      <c r="Q13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
-      <c r="I14" s="20" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="17" t="n">
-        <f aca="false">I8/J8</f>
+      <c r="K14" s="17" t="n">
+        <f aca="false">J8/K8</f>
         <v>7.74214057872503</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="M14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M14" s="18" t="n">
-        <f aca="false">L8/M8</f>
+      <c r="N14" s="18" t="n">
+        <f aca="false">M8/N8</f>
         <v>-6.41507800470515</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="P14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="P14" s="18" t="n">
-        <f aca="false">O8/P8</f>
+      <c r="Q14" s="18" t="n">
+        <f aca="false">P8/Q8</f>
         <v>17943147791341.7</v>
       </c>
-      <c r="Q14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
-      <c r="I15" s="20" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="17" t="n">
-        <f aca="false">I9/J9</f>
+      <c r="K15" s="17" t="n">
+        <f aca="false">J9/K9</f>
         <v>-2.57982287259323</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="M15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="18" t="n">
-        <f aca="false">L9/M9</f>
+      <c r="N15" s="18" t="n">
+        <f aca="false">M9/N9</f>
         <v>2.1004535114573</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="P15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="18" t="n">
-        <f aca="false">O9/P9</f>
+      <c r="Q15" s="18" t="n">
+        <f aca="false">P9/Q9</f>
         <v>16872101695923.6</v>
       </c>
-      <c r="Q15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
-      <c r="Q16" s="0"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
-      <c r="G17" s="0"/>
-      <c r="H17" s="0"/>
-      <c r="I17" s="6" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="K17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="N17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O17" s="6" t="s">
+      <c r="P17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="Q17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="Q17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0"/>
-      <c r="J18" s="21"/>
-      <c r="L18" s="0"/>
-      <c r="M18" s="21"/>
-      <c r="O18" s="19" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="K18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="P18" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="P18" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(P12),$O$24)</f>
+      <c r="Q18" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(Q12),$P$25)</f>
         <v>2.83474932235218E-131</v>
       </c>
-      <c r="Q18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
-      <c r="J19" s="21"/>
-      <c r="L19" s="20" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="K19" s="21"/>
+      <c r="M19" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M19" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(M13),$L$24)</f>
+      <c r="N19" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(N13),$M$25)</f>
         <v>3.15348246062016E-009</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="P19" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(P13),$O$24)</f>
+      <c r="Q19" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(Q13),$P$25)</f>
         <v>1.6835402615869E-121</v>
       </c>
-      <c r="Q19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
-      <c r="G20" s="0"/>
-      <c r="H20" s="0"/>
-      <c r="I20" s="20" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(J14),$I$24)</f>
+      <c r="K20" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(K14),$J$25)</f>
         <v>8.90736413654872E-006</v>
       </c>
-      <c r="L20" s="20" t="s">
+      <c r="M20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(M14),$L$24)</f>
+      <c r="N20" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(N14),$M$25)</f>
         <v>7.68281202590709E-005</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="P20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="P20" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(P14),$O$24)</f>
+      <c r="Q20" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(Q14),$P$25)</f>
         <v>2.6410895255234E-116</v>
       </c>
-      <c r="Q20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
-      <c r="H21" s="0"/>
-      <c r="I21" s="20" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="J21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(J15),$I$24)</f>
+      <c r="K21" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(K15),$J$25)</f>
         <v>0.0255983855295941</v>
       </c>
-      <c r="L21" s="20" t="s">
+      <c r="M21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(M15),$L$24)</f>
+      <c r="N21" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(N15),$M$25)</f>
         <v>0.0620299422471254</v>
       </c>
-      <c r="O21" s="20" t="s">
+      <c r="P21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="P21" s="21" t="n">
-        <f aca="false">_xlfn.T.DIST.2T(ABS(P15),$O$24)</f>
+      <c r="Q21" s="21" t="n">
+        <f aca="false">_xlfn.T.DIST.2T(ABS(Q15),$P$25)</f>
         <v>4.59566296878242E-116</v>
       </c>
-      <c r="Q21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="5" t="s">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="25"/>
+    </row>
+    <row r="23" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="F23" s="5" t="s">
+      <c r="C24" s="5"/>
+      <c r="G24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="I23" s="22" t="s">
+      <c r="H24" s="5"/>
+      <c r="J24" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="K24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="M24" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="N24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="O23" s="24" t="s">
+      <c r="P24" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="P23" s="6" t="s">
+      <c r="Q24" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-      <c r="G24" s="0"/>
-      <c r="I24" s="25" t="n">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="29" t="n">
         <f aca="false">COUNT(x_observed)-2</f>
         <v>11</v>
       </c>
-      <c r="J24" s="26" t="n">
-        <f aca="false" t="array" ref="J24:J24">SUMSQ(y_observed-y1_predicted)</f>
+      <c r="K25" s="30" t="n">
+        <f aca="false" t="array" ref="K25:K25">SUMSQ(y_observed-y1_predicted)</f>
         <v>3127410</v>
       </c>
-      <c r="L24" s="27" t="n">
+      <c r="M25" s="29" t="n">
         <f aca="false">COUNT(x_observed)-3</f>
         <v>10</v>
       </c>
-      <c r="M24" s="26" t="n">
-        <f aca="false" t="array" ref="M24:M24">SUMSQ(y_observed-y2_predicted)</f>
+      <c r="N25" s="30" t="n">
+        <f aca="false" t="array" ref="N25:N25">SUMSQ(y_observed-y2_predicted)</f>
         <v>82368.0000000001</v>
       </c>
-      <c r="O24" s="28" t="n">
+      <c r="P25" s="29" t="n">
         <f aca="false">COUNT(x_observed)-4</f>
         <v>9</v>
       </c>
-      <c r="P24" s="26" t="n">
-        <f aca="false" t="array" ref="P24:P24">SUMSQ(y_observed-y3_predicted)</f>
+      <c r="Q25" s="30" t="n">
+        <f aca="false" t="array" ref="Q25:Q25">SUMSQ(y_observed-y3_predicted)</f>
         <v>1.34346167602759E-025</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="0"/>
-      <c r="J25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="P25" s="26"/>
-    </row>
-    <row r="26" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="K26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="Q26" s="30"/>
+    </row>
+    <row r="27" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="0"/>
-      <c r="I27" s="16" t="s">
+      <c r="C28" s="16"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="J28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="L27" s="16" t="s">
+      <c r="K28" s="16"/>
+      <c r="M28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="16"/>
-      <c r="O27" s="16" t="s">
+      <c r="N28" s="16"/>
+      <c r="P28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P27" s="16"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="22" t="s">
+      <c r="Q28" s="16"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C29" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="16" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="J29" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="K29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="6" t="s">
+      <c r="M29" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="M28" s="16" t="s">
+      <c r="N29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="O28" s="6" t="s">
+      <c r="P29" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="P28" s="16" t="s">
+      <c r="Q29" s="32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="25" t="n">
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="29" t="n">
         <f aca="false">COUNT(x_observed)</f>
         <v>13</v>
       </c>
-      <c r="C29" s="28" t="n">
-        <f aca="false" t="array" ref="C29:C29">COUNT(x_observed)</f>
+      <c r="C30" s="33" t="n">
+        <f aca="false" t="array" ref="C30:C30">COUNT(x_observed)</f>
         <v>13</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26" t="n">
-        <f aca="false" t="array" ref="G29:G29">SUMSQ(y_observed-$C$33)</f>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30" t="n">
+        <f aca="false" t="array" ref="H30:H30">SUMSQ(y_observed-$C$34)</f>
         <v>20169162</v>
       </c>
-      <c r="I29" s="31" t="n">
-        <f aca="false">1-($J$24/$G$29)</f>
+      <c r="J30" s="34" t="n">
+        <f aca="false">1-($K$25/$H$30)</f>
         <v>0.844941004489924</v>
       </c>
-      <c r="J29" s="31" t="n">
-        <f aca="false">1-((1-I29)*($B$29-1)/$I24)</f>
+      <c r="K30" s="35" t="n">
+        <f aca="false">1-((1-J30)*($B$30-1)/$J25)</f>
         <v>0.830844732170826</v>
       </c>
-      <c r="L29" s="31" t="n">
-        <f aca="false">1-($M$24/$G$29)</f>
+      <c r="M30" s="34" t="n">
+        <f aca="false">1-($N$25/$H$30)</f>
         <v>0.995916141682039</v>
       </c>
-      <c r="M29" s="31" t="n">
-        <f aca="false">1-((1-L29)*($B$29-1)/$I24)</f>
+      <c r="N30" s="35" t="n">
+        <f aca="false">1-((1-M30)*($B$30-1)/$J25)</f>
         <v>0.995544881834952</v>
       </c>
-      <c r="O29" s="31" t="n">
-        <f aca="false">1-($P$24/$G$29)</f>
+      <c r="P30" s="34" t="n">
+        <f aca="false">1-($Q$25/$H$30)</f>
         <v>1</v>
       </c>
-      <c r="P29" s="31" t="n">
-        <f aca="false">1-((1-O29)*($B$29-1)/$I24)</f>
+      <c r="Q30" s="35" t="n">
+        <f aca="false">1-((1-P30)*($B$30-1)/$J25)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="16" t="s">
+    <row r="31" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="I31" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="L31" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M31" s="16"/>
-      <c r="O31" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="P31" s="16"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="C32" s="16"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="I32" s="6" t="s">
+      <c r="G32" s="2"/>
+      <c r="J32" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K32" s="16"/>
+      <c r="M32" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N32" s="16"/>
+      <c r="P32" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q32" s="16"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="J33" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J32" s="16" t="s">
+      <c r="K33" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="M33" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="M32" s="16" t="s">
+      <c r="N33" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="O32" s="6" t="s">
+      <c r="P33" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="P32" s="16" t="s">
+      <c r="Q33" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="32" t="n">
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="36" t="n">
         <f aca="false">AVERAGE(x_observed)</f>
         <v>6</v>
       </c>
-      <c r="C33" s="33" t="n">
+      <c r="C34" s="37" t="n">
         <f aca="false">AVERAGE(y_observed)</f>
         <v>1115</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="I33" s="26" t="n">
-        <f aca="false">J24/$I$24</f>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="29" t="n">
+        <f aca="false">K25/$J$25</f>
         <v>284310</v>
       </c>
-      <c r="J33" s="34" t="n">
-        <f aca="false">SQRT(I33)</f>
+      <c r="K34" s="37" t="n">
+        <f aca="false">SQRT(J34)</f>
         <v>533.207276769551</v>
       </c>
-      <c r="L33" s="26" t="n">
-        <f aca="false">M24/$L$24</f>
+      <c r="M34" s="34" t="n">
+        <f aca="false">N25/$M$25</f>
         <v>8236.80000000001</v>
       </c>
-      <c r="M33" s="34" t="n">
-        <f aca="false">SQRT(L33)</f>
+      <c r="N34" s="35" t="n">
+        <f aca="false">SQRT(M34)</f>
         <v>90.7568179257074</v>
       </c>
-      <c r="O33" s="26" t="n">
-        <f aca="false">P24/$O$24</f>
+      <c r="P34" s="34" t="n">
+        <f aca="false">Q25/$P$25</f>
         <v>1.49273519558621E-026</v>
       </c>
-      <c r="P33" s="34" t="n">
-        <f aca="false">SQRT(O33)</f>
+      <c r="Q34" s="35" t="n">
+        <f aca="false">SQRT(P34)</f>
         <v>1.22177542764054E-013</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="39"/>
-    </row>
     <row r="35" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="41"/>
-      <c r="O35" s="41"/>
-      <c r="P35" s="41"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="5" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="25"/>
+    </row>
+    <row r="36" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+    </row>
+    <row r="37" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="E36" s="5" t="s">
+      <c r="C38" s="5"/>
+      <c r="E38" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="42" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="H38" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E37" s="43" t="s">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E39" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="43" t="s">
+      <c r="F39" s="41"/>
+      <c r="G39" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="43" t="s">
+      <c r="H39" s="41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="44" t="s">
+    <row r="40" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="E39" s="44" t="s">
+      <c r="C41" s="42"/>
+      <c r="E41" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="22" t="s">
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C42" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E42" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F42" s="43"/>
+      <c r="G42" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="47" t="s">
+      <c r="H42" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="48" t="n">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="46" t="n">
         <v>0</v>
       </c>
-      <c r="C41" s="28" t="n">
+      <c r="C43" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="E41" s="34" t="n">
-        <f aca="false" t="array" ref="E41:E41">SUMPRODUCT(TRANSPOSE(coeff_1),B41^{1,0})</f>
+      <c r="E43" s="47" t="n">
+        <f aca="false" t="array" ref="E43:E43">SUMPRODUCT(TRANSPOSE(coeff_1),B43^{1,0})</f>
         <v>-721</v>
       </c>
-      <c r="F41" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B41^{2,1,0})</f>
+      <c r="F43" s="47"/>
+      <c r="G43" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B43^{2,1,0})</f>
         <v>137</v>
       </c>
-      <c r="G41" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B41^{3,2,1,0})</f>
+      <c r="H43" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B43^{3,2,1,0})</f>
         <v>5.00000000000023</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="48" t="n">
-        <f aca="false">B41+1</f>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="46" t="n">
+        <f aca="false">B43+1</f>
         <v>1</v>
       </c>
-      <c r="C42" s="28" t="n">
+      <c r="C44" s="33" t="n">
         <v>14</v>
       </c>
-      <c r="E42" s="34" t="n">
-        <f aca="false" t="array" ref="E42:E42">SUMPRODUCT(TRANSPOSE(coeff_1),B42^{1,0})</f>
+      <c r="E44" s="47" t="n">
+        <f aca="false" t="array" ref="E44:E44">SUMPRODUCT(TRANSPOSE(coeff_1),B44^{1,0})</f>
         <v>-415</v>
       </c>
-      <c r="F42" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B42^{2,1,0})</f>
+      <c r="F44" s="47"/>
+      <c r="G44" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B44^{2,1,0})</f>
         <v>14.0000000000003</v>
       </c>
-      <c r="G42" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B42^{3,2,1,0})</f>
+      <c r="H44" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B44^{3,2,1,0})</f>
         <v>14.0000000000002</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="48" t="n">
-        <f aca="false">B42+1</f>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="46" t="n">
+        <f aca="false">B44+1</f>
         <v>2</v>
       </c>
-      <c r="C43" s="28" t="n">
+      <c r="C45" s="33" t="n">
         <v>41</v>
       </c>
-      <c r="E43" s="34" t="n">
-        <f aca="false" t="array" ref="E43:E43">SUMPRODUCT(TRANSPOSE(coeff_1),B43^{1,0})</f>
+      <c r="E45" s="47" t="n">
+        <f aca="false" t="array" ref="E45:E45">SUMPRODUCT(TRANSPOSE(coeff_1),B45^{1,0})</f>
         <v>-109</v>
       </c>
-      <c r="F43" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B43^{2,1,0})</f>
+      <c r="F45" s="47"/>
+      <c r="G45" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B45^{2,1,0})</f>
         <v>-30.9999999999998</v>
       </c>
-      <c r="G43" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B43^{3,2,1,0})</f>
+      <c r="H45" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B45^{3,2,1,0})</f>
         <v>41.0000000000002</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="48" t="n">
-        <f aca="false">B43+1</f>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="46" t="n">
+        <f aca="false">B45+1</f>
         <v>3</v>
       </c>
-      <c r="C44" s="28" t="n">
+      <c r="C46" s="33" t="n">
         <v>98</v>
       </c>
-      <c r="E44" s="34" t="n">
-        <f aca="false" t="array" ref="E44:E44">SUMPRODUCT(TRANSPOSE(coeff_1),B44^{1,0})</f>
+      <c r="E46" s="47" t="n">
+        <f aca="false" t="array" ref="E46:E46">SUMPRODUCT(TRANSPOSE(coeff_1),B46^{1,0})</f>
         <v>197</v>
       </c>
-      <c r="F44" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B44^{2,1,0})</f>
+      <c r="F46" s="47"/>
+      <c r="G46" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B46^{2,1,0})</f>
         <v>2.00000000000017</v>
       </c>
-      <c r="G44" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B44^{3,2,1,0})</f>
+      <c r="H46" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B46^{3,2,1,0})</f>
         <v>98.0000000000001</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="48" t="n">
-        <f aca="false">B44+1</f>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="46" t="n">
+        <f aca="false">B46+1</f>
         <v>4</v>
       </c>
-      <c r="C45" s="28" t="n">
+      <c r="C47" s="33" t="n">
         <v>197</v>
       </c>
-      <c r="E45" s="34" t="n">
-        <f aca="false" t="array" ref="E45:E45">SUMPRODUCT(TRANSPOSE(coeff_1),B45^{1,0})</f>
+      <c r="E47" s="47" t="n">
+        <f aca="false" t="array" ref="E47:E47">SUMPRODUCT(TRANSPOSE(coeff_1),B47^{1,0})</f>
         <v>503</v>
       </c>
-      <c r="F45" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B45^{2,1,0})</f>
+      <c r="F47" s="47"/>
+      <c r="G47" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B47^{2,1,0})</f>
         <v>113</v>
       </c>
-      <c r="G45" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B45^{3,2,1,0})</f>
+      <c r="H47" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B47^{3,2,1,0})</f>
         <v>197</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="48" t="n">
-        <f aca="false">B45+1</f>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="46" t="n">
+        <f aca="false">B47+1</f>
         <v>5</v>
       </c>
-      <c r="C46" s="28" t="n">
+      <c r="C48" s="33" t="n">
         <v>350</v>
       </c>
-      <c r="E46" s="34" t="n">
-        <f aca="false" t="array" ref="E46:E46">SUMPRODUCT(TRANSPOSE(coeff_1),B46^{1,0})</f>
+      <c r="E48" s="47" t="n">
+        <f aca="false" t="array" ref="E48:E48">SUMPRODUCT(TRANSPOSE(coeff_1),B48^{1,0})</f>
         <v>809</v>
       </c>
-      <c r="F46" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B46^{2,1,0})</f>
+      <c r="F48" s="47"/>
+      <c r="G48" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B48^{2,1,0})</f>
         <v>302</v>
       </c>
-      <c r="G46" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B46^{3,2,1,0})</f>
+      <c r="H48" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B48^{3,2,1,0})</f>
         <v>350</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="48" t="n">
-        <f aca="false">B46+1</f>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="46" t="n">
+        <f aca="false">B48+1</f>
         <v>6</v>
       </c>
-      <c r="C47" s="28" t="n">
+      <c r="C49" s="33" t="n">
         <v>569</v>
       </c>
-      <c r="E47" s="34" t="n">
-        <f aca="false" t="array" ref="E47:E47">SUMPRODUCT(TRANSPOSE(coeff_1),B47^{1,0})</f>
+      <c r="E49" s="47" t="n">
+        <f aca="false" t="array" ref="E49:E49">SUMPRODUCT(TRANSPOSE(coeff_1),B49^{1,0})</f>
         <v>1115</v>
       </c>
-      <c r="F47" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B47^{2,1,0})</f>
+      <c r="F49" s="47"/>
+      <c r="G49" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B49^{2,1,0})</f>
         <v>569</v>
       </c>
-      <c r="G47" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B47^{3,2,1,0})</f>
+      <c r="H49" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B49^{3,2,1,0})</f>
         <v>569</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="48" t="n">
-        <f aca="false">B47+1</f>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="46" t="n">
+        <f aca="false">B49+1</f>
         <v>7</v>
       </c>
-      <c r="C48" s="28" t="n">
+      <c r="C50" s="33" t="n">
         <v>866</v>
       </c>
-      <c r="E48" s="34" t="n">
-        <f aca="false" t="array" ref="E48:E48">SUMPRODUCT(TRANSPOSE(coeff_1),B48^{1,0})</f>
+      <c r="E50" s="47" t="n">
+        <f aca="false" t="array" ref="E50:E50">SUMPRODUCT(TRANSPOSE(coeff_1),B50^{1,0})</f>
         <v>1421</v>
       </c>
-      <c r="F48" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B48^{2,1,0})</f>
+      <c r="F50" s="47"/>
+      <c r="G50" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B50^{2,1,0})</f>
         <v>914</v>
       </c>
-      <c r="G48" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B48^{3,2,1,0})</f>
+      <c r="H50" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B50^{3,2,1,0})</f>
         <v>866</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="48" t="n">
-        <f aca="false">B48+1</f>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="46" t="n">
+        <f aca="false">B50+1</f>
         <v>8</v>
       </c>
-      <c r="C49" s="28" t="n">
+      <c r="C51" s="33" t="n">
         <v>1253</v>
       </c>
-      <c r="E49" s="34" t="n">
-        <f aca="false" t="array" ref="E49:E49">SUMPRODUCT(TRANSPOSE(coeff_1),B49^{1,0})</f>
+      <c r="E51" s="47" t="n">
+        <f aca="false" t="array" ref="E51:E51">SUMPRODUCT(TRANSPOSE(coeff_1),B51^{1,0})</f>
         <v>1727</v>
       </c>
-      <c r="F49" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B49^{2,1,0})</f>
+      <c r="F51" s="47"/>
+      <c r="G51" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B51^{2,1,0})</f>
         <v>1337</v>
       </c>
-      <c r="G49" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B49^{3,2,1,0})</f>
+      <c r="H51" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B51^{3,2,1,0})</f>
         <v>1253</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="48" t="n">
-        <f aca="false">B49+1</f>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="46" t="n">
+        <f aca="false">B51+1</f>
         <v>9</v>
       </c>
-      <c r="C50" s="28" t="n">
+      <c r="C52" s="33" t="n">
         <v>1742</v>
       </c>
-      <c r="E50" s="34" t="n">
-        <f aca="false" t="array" ref="E50:E50">SUMPRODUCT(TRANSPOSE(coeff_1),B50^{1,0})</f>
+      <c r="E52" s="47" t="n">
+        <f aca="false" t="array" ref="E52:E52">SUMPRODUCT(TRANSPOSE(coeff_1),B52^{1,0})</f>
         <v>2033</v>
       </c>
-      <c r="F50" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B50^{2,1,0})</f>
+      <c r="F52" s="47"/>
+      <c r="G52" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B52^{2,1,0})</f>
         <v>1838</v>
       </c>
-      <c r="G50" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B50^{3,2,1,0})</f>
+      <c r="H52" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B52^{3,2,1,0})</f>
         <v>1742</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="48" t="n">
-        <f aca="false">B50+1</f>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="46" t="n">
+        <f aca="false">B52+1</f>
         <v>10</v>
       </c>
-      <c r="C51" s="28" t="n">
+      <c r="C53" s="33" t="n">
         <v>2345</v>
       </c>
-      <c r="E51" s="34" t="n">
-        <f aca="false" t="array" ref="E51:E51">SUMPRODUCT(TRANSPOSE(coeff_1),B51^{1,0})</f>
+      <c r="E53" s="47" t="n">
+        <f aca="false" t="array" ref="E53:E53">SUMPRODUCT(TRANSPOSE(coeff_1),B53^{1,0})</f>
         <v>2339</v>
       </c>
-      <c r="F51" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B51^{2,1,0})</f>
+      <c r="F53" s="47"/>
+      <c r="G53" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B53^{2,1,0})</f>
         <v>2417</v>
       </c>
-      <c r="G51" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B51^{3,2,1,0})</f>
+      <c r="H53" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B53^{3,2,1,0})</f>
         <v>2345</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="48" t="n">
-        <f aca="false">B51+1</f>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="46" t="n">
+        <f aca="false">B53+1</f>
         <v>11</v>
       </c>
-      <c r="C52" s="28" t="n">
+      <c r="C54" s="33" t="n">
         <v>3074</v>
       </c>
-      <c r="E52" s="34" t="n">
-        <f aca="false" t="array" ref="E52:E52">SUMPRODUCT(TRANSPOSE(coeff_1),B52^{1,0})</f>
+      <c r="E54" s="47" t="n">
+        <f aca="false" t="array" ref="E54:E54">SUMPRODUCT(TRANSPOSE(coeff_1),B54^{1,0})</f>
         <v>2645</v>
       </c>
-      <c r="F52" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B52^{2,1,0})</f>
+      <c r="F54" s="47"/>
+      <c r="G54" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B54^{2,1,0})</f>
         <v>3074</v>
       </c>
-      <c r="G52" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B52^{3,2,1,0})</f>
+      <c r="H54" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B54^{3,2,1,0})</f>
         <v>3074</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="48" t="n">
-        <f aca="false">B52+1</f>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="46" t="n">
+        <f aca="false">B54+1</f>
         <v>12</v>
       </c>
-      <c r="C53" s="28" t="n">
+      <c r="C55" s="33" t="n">
         <v>3941</v>
       </c>
-      <c r="E53" s="34" t="n">
-        <f aca="false" t="array" ref="E53:E53">SUMPRODUCT(TRANSPOSE(coeff_1),B53^{1,0})</f>
+      <c r="E55" s="47" t="n">
+        <f aca="false" t="array" ref="E55:E55">SUMPRODUCT(TRANSPOSE(coeff_1),B55^{1,0})</f>
         <v>2951</v>
       </c>
-      <c r="F53" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B53^{2,1,0})</f>
+      <c r="F55" s="47"/>
+      <c r="G55" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_2),B55^{2,1,0})</f>
         <v>3809</v>
       </c>
-      <c r="G53" s="33" t="n">
-        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B53^{3,2,1,0})</f>
+      <c r="H55" s="37" t="n">
+        <f aca="false">SUMPRODUCT(TRANSPOSE(coeff_3),B55^{3,2,1,0})</f>
         <v>3941</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="8.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="E41:H41"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>